<commit_message>
chem101 mid-1+mid-2 papers updated Commit by @arfazhxss on Fri 14 Jun 2024
</commit_message>
<xml_diff>
--- a/1 Summer 2024/1 CHEM 101 A01 B01/0 Labs/0 Past Submissions/Lab4/Book1.xlsx
+++ b/1 Summer 2024/1 CHEM 101 A01 B01/0 Labs/0 Past Submissions/Lab4/Book1.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvic-my.sharepoint.com/personal/arfazhussain_uvic_ca/Documents/0 UVIC/2 ENGR Y3/2 CHEM 101 A02 B12/1 Lab/Lab4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arfaz/Desktop/ThirdYearEngineering/1 Summer 2024/1 CHEM 101 A01 B01/0 Labs/0 Past Submissions/Lab4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{8541EEF4-93C0-1B4B-A7B9-5301D6C51424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68EA4A89-53FB-2340-BE4B-5DCA534D4612}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B75EAF-0E5D-1F48-A6DC-053FC8F98D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="37400" windowHeight="21100" xr2:uid="{EB1F210C-BB4B-8141-9EF5-4BD3C8FB5D43}"/>
+    <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{EB1F210C-BB4B-8141-9EF5-4BD3C8FB5D43}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,22 +38,124 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Concentration (mmole/L)</t>
   </si>
   <si>
     <t>Absorbances</t>
   </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Volume of acne cleanser used in the analysis (mL)</t>
+  </si>
+  <si>
+    <t>0.3mL</t>
+  </si>
+  <si>
+    <t>Density of the acne cleanser used in the analysis (g/cm3)</t>
+  </si>
+  <si>
+    <t>Advertised %mass of salicylic acid</t>
+  </si>
+  <si>
+    <t>Aliquot #1</t>
+  </si>
+  <si>
+    <t>Aliquot #2</t>
+  </si>
+  <si>
+    <t>Aliquot #3</t>
+  </si>
+  <si>
+    <t>Maximum absorbance at 535 nm</t>
+  </si>
+  <si>
+    <t>[salicylic acid] from the curve (M)</t>
+  </si>
+  <si>
+    <t>Moles of salicylic acid in 25.00 mL (mol)</t>
+  </si>
+  <si>
+    <t>Mass of salicylic acid in 25.00 mL (g)</t>
+  </si>
+  <si>
+    <t>Initial concentration of salicylic acid before dilation (M)</t>
+  </si>
+  <si>
+    <t>Moles of salicylic acid in 1.00 mL of acne cleanser (mole)</t>
+  </si>
+  <si>
+    <t>Mass of salicylic acid in 1.00 mL of acne cleanser (g)</t>
+  </si>
+  <si>
+    <t>%mass of salicylic acid in acne cleanser</t>
+  </si>
+  <si>
+    <t>Average % mass of salicylic acid in acne cleanser</t>
+  </si>
+  <si>
+    <t>Standard deviation of average % mass</t>
+  </si>
+  <si>
+    <t>% RSD</t>
+  </si>
+  <si>
+    <t>% comparison to the advertised value</t>
+  </si>
+  <si>
+    <t>Concentration (mole/L)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="5">
+    <numFmt numFmtId="168" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="171" formatCode="0.000000000E+00"/>
+    <numFmt numFmtId="193" formatCode="0.0000000000"/>
+    <numFmt numFmtId="201" formatCode="0.00000000%"/>
+    <numFmt numFmtId="202" formatCode="0.000000000%"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -65,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -73,14 +177,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="202" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="193" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="193" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="193" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="193" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="201" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="201" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="201" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -120,9 +345,373 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1650" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1650" b="0"/>
+              <a:t>Spectrophotometric determination of Fe (II) Complexes at 535 nm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13655761339691691"/>
+          <c:y val="3.6674816625916873E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1650" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14215412554064544"/>
+          <c:y val="0.12624169986719788"/>
+          <c:w val="0.79321697903959187"/>
+          <c:h val="0.6663234699574534"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$H$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.1142</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1142</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57099999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57099999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1419999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.151</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.73599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3620000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.363</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-1CD5-1849-9FC0-F9310A436DB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$H$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.1142</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1142</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57099999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57099999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1419999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$H$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.151</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.73599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3620000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.363</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1CD5-1849-9FC0-F9310A436DB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="395478784"/>
+        <c:axId val="395480496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="395478784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -132,18 +721,581 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="395480496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="395480496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="395478784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1650" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Spectrophotometric</a:t>
+              <a:rPr lang="en-US" sz="1650" b="0"/>
+              <a:t>Spectrophotometric determination of Fe (II) Complexes at 535 nm</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> determination of Fe (II) Complexes at 535 nm</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13095775154643455"/>
+          <c:y val="5.2914107234305875E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1650" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12118868793303354"/>
+          <c:y val="0.12896966759035386"/>
+          <c:w val="0.81661476201613226"/>
+          <c:h val="0.69141492612585587"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.142E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.142E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.142E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.71E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.71E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.142E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.142E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.151</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.73599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3620000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.363</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6069-3642-B472-45B3DF796392}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="655818352"/>
+        <c:axId val="655820064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="655818352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="655820064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="655820064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="655818352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -182,17 +1334,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Absorbances</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -231,45 +1372,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.9797401952583206E-2"/>
-                  <c:y val="-1.6794496841740936E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="65000"/>
-                            <a:lumOff val="35000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                      <a:t>y = 0.0429x + 0.0863</a:t>
-                    </a:r>
-                    <a:br>
-                      <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                    </a:br>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                      <a:t>R² = 0.9965</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="1600"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -302,42 +1404,36 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:f>Sheet3!$C$10:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.9159999999999999</c:v>
+                  <c:v>0.11668000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.58</c:v>
+                  <c:v>0.58340000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.16</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.8997668999999995</c:v>
+                  <c:v>1.1668000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$E$2</c:f>
+              <c:f>Sheet3!$C$11:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.19</c:v>
+                  <c:v>0.24399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.751</c:v>
+                  <c:v>0.83099999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.321</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.51100000000000001</c:v>
+                  <c:v>1.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -345,7 +1441,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C87D-9E4C-8EC4-3E1F8FB42633}"/>
+              <c16:uniqueId val="{00000000-EF97-9A42-8A90-0BC8C77CC3A2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -357,11 +1453,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71020704"/>
-        <c:axId val="1905753488"/>
+        <c:axId val="654620480"/>
+        <c:axId val="1311184207"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71020704"/>
+        <c:axId val="654620480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,12 +1514,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1905753488"/>
+        <c:crossAx val="1311184207"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1905753488"/>
+        <c:axId val="1311184207"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,7 +1576,358 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71020704"/>
+        <c:crossAx val="654620480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$C$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.1668E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8339999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1668E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$C$13:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.24399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DCE5-E74F-B5E9-26AC67BF2CBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="667776143"/>
+        <c:axId val="667777855"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="667776143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="667777855"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="667777855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="667776143"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -576,7 +2023,1279 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="250">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="250">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1092,27 +3811,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>501650</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{897C6F0B-0543-12EE-6CD0-FD66F8F4ACD1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02D113C6-38B2-1A2A-A313-D5C0EFFA2ADD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1130,17 +4365,460 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1841500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>182032</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>12699</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94257E0B-2B73-4B6F-5804-7E7C4F31020D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.18936</cdr:x>
+      <cdr:y>0.86797</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.84986</cdr:x>
+      <cdr:y>0.95599</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{869EFB29-FB50-A1B5-E9EC-C2573628E5D2}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1365965" y="4508500"/>
+          <a:ext cx="4764613" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="2000">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Concentration (nmole/L) of Standard</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> Solutions</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>  </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.03538</cdr:x>
+      <cdr:y>0.32763</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.09756</cdr:x>
+      <cdr:y>0.60147</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFE44B8B-D711-F9D2-B782-E3C93CBDB1D4}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
+          <a:off x="-231715" y="2188711"/>
+          <a:ext cx="1422400" cy="448577"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="2000">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Absorbance</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.01167</cdr:x>
+      <cdr:y>0.39418</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.07382</cdr:x>
+      <cdr:y>0.64502</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="8" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0179D98F-0234-1A40-F13F-855B4C1A6D92}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
+          <a:off x="-401061" y="2720927"/>
+          <a:ext cx="1422400" cy="450946"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="2000">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Absorbance</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.18436</cdr:x>
+      <cdr:y>0.87794</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.84448</cdr:x>
+      <cdr:y>0.95857</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69081777-19FD-74AE-E2B1-2E9C08DFF876}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1337734" y="4978400"/>
+          <a:ext cx="4789778" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="2000">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Concentration (mole/L) of Standard</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> Solutions</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>  </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9629810A-CCFC-7E34-58D1-DA1DDD50FDD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25A9C43E-0364-78B0-F268-BA8BDB5D8C1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1178,7 +4856,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1284,7 +4962,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1426,61 +5104,542 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E4585BD-463C-534E-83B3-7D00CDAC0563}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17235206-13E0-F444-8427-08B45CA9E427}">
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>2.9159999999999999</v>
+        <f>B3*1000</f>
+        <v>0.1142</v>
       </c>
       <c r="C1">
-        <v>14.58</v>
+        <f>C3*1000</f>
+        <v>0.1142</v>
       </c>
       <c r="D1">
-        <v>29.16</v>
+        <f>D3*1000</f>
+        <v>0.1142</v>
       </c>
       <c r="E1">
-        <v>9.8997668999999995</v>
+        <f>E3*1000</f>
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="F1">
+        <f>F3*1000</f>
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="G1">
+        <f>G3*1000</f>
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="H1">
+        <f>H3*1000</f>
+        <v>1.1419999999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.19</v>
+        <v>0.151</v>
       </c>
       <c r="C2">
-        <v>0.751</v>
+        <v>0.152</v>
       </c>
       <c r="D2">
-        <v>1.321</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.51100000000000001</v>
+        <v>0.154</v>
+      </c>
+      <c r="E2">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="F2">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1.3620000000000001</v>
+      </c>
+      <c r="H2">
+        <v>1.363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>1.142E-4</v>
+      </c>
+      <c r="C3">
+        <v>1.142E-4</v>
+      </c>
+      <c r="D3">
+        <v>1.142E-4</v>
+      </c>
+      <c r="E3">
+        <v>5.71E-4</v>
+      </c>
+      <c r="F3">
+        <v>5.71E-4</v>
+      </c>
+      <c r="G3">
+        <v>1.142E-3</v>
+      </c>
+      <c r="H3">
+        <v>1.142E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.151</v>
+      </c>
+      <c r="C4">
+        <v>0.152</v>
+      </c>
+      <c r="D4">
+        <v>0.154</v>
+      </c>
+      <c r="E4">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1.3620000000000001</v>
+      </c>
+      <c r="H4">
+        <v>1.363</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>0.624</v>
+      </c>
+      <c r="C12">
+        <v>0.621</v>
+      </c>
+      <c r="D12">
+        <v>0.623</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <f>(B12-0.0298)/1179.8</f>
+        <v>5.0364468553992195E-4</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:D13" si="0">(C12-0.0298)/1179.8</f>
+        <v>5.0110188167486007E-4</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>5.0279708425156799E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0254B03C-B6C9-9643-B033-6429E6DAA021}">
+  <dimension ref="C10:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f>C12*1000</f>
+        <v>0.11668000000000001</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:E10" si="0">D12*1000</f>
+        <v>0.58340000000000003</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.1668000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="E11">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>1.1668E-4</v>
+      </c>
+      <c r="D12">
+        <v>5.8339999999999998E-4</v>
+      </c>
+      <c r="E12">
+        <v>1.1668E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="D13">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="E13">
+        <v>1.39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C8A8A2-45DA-314B-8906-9F00CCC87B7A}">
+  <dimension ref="A2:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="12"/>
+    <col min="2" max="2" width="29" style="12" customWidth="1"/>
+    <col min="3" max="5" width="13.5" style="12" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11"/>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="3">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.624</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.621</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.623</v>
+      </c>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="19">
+        <f>(C7-0.0298)/1179.8</f>
+        <v>5.0364468553992195E-4</v>
+      </c>
+      <c r="D8" s="20">
+        <f t="shared" ref="D8:E8" si="0">(D7-0.0298)/1179.8</f>
+        <v>5.0110188167486007E-4</v>
+      </c>
+      <c r="E8" s="20">
+        <f t="shared" si="0"/>
+        <v>5.0279708425156799E-4</v>
+      </c>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="18">
+        <f>C8*(25/1000)</f>
+        <v>1.2591117138498049E-5</v>
+      </c>
+      <c r="D9" s="18">
+        <f>D8*(25/1000)</f>
+        <v>1.2527547041871502E-5</v>
+      </c>
+      <c r="E9" s="18">
+        <f>E8*(25/1000)</f>
+        <v>1.2569927106289201E-5</v>
+      </c>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="18">
+        <f>C9*138.1214</f>
+        <v>1.7391027267333445E-3</v>
+      </c>
+      <c r="D10" s="18">
+        <f t="shared" ref="D10:E10" si="1">D9*138.1214</f>
+        <v>1.7303223359891504E-3</v>
+      </c>
+      <c r="E10" s="18">
+        <f t="shared" si="1"/>
+        <v>1.7361759298186131E-3</v>
+      </c>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="21">
+        <f>C9/(0.3/1000)</f>
+        <v>4.1970390461660165E-2</v>
+      </c>
+      <c r="D11" s="21">
+        <f t="shared" ref="D11:E11" si="2">D9/(0.3/1000)</f>
+        <v>4.1758490139571676E-2</v>
+      </c>
+      <c r="E11" s="21">
+        <f t="shared" si="2"/>
+        <v>4.1899757020964011E-2</v>
+      </c>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="13">
+        <f>C11*(1/1000)</f>
+        <v>4.1970390461660163E-5</v>
+      </c>
+      <c r="D12" s="13">
+        <f t="shared" ref="D12:E12" si="3">D11*(1/1000)</f>
+        <v>4.1758490139571679E-5</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="3"/>
+        <v>4.1899757020964015E-5</v>
+      </c>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="18">
+        <f>C12*138.1214</f>
+        <v>5.7970090891111478E-3</v>
+      </c>
+      <c r="D13" s="18">
+        <f t="shared" ref="D13:E13" si="4">D12*138.1214</f>
+        <v>5.7677411199638356E-3</v>
+      </c>
+      <c r="E13" s="18">
+        <f t="shared" si="4"/>
+        <v>5.7872530993953791E-3</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="17">
+        <f>C13/$D4</f>
+        <v>6.0322675224881873E-3</v>
+      </c>
+      <c r="D14" s="17">
+        <f t="shared" ref="D14:E14" si="5">D13/$D4</f>
+        <v>6.0018117793588302E-3</v>
+      </c>
+      <c r="E14" s="17">
+        <f t="shared" si="5"/>
+        <v>6.0221156081117369E-3</v>
+      </c>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11"/>
+      <c r="B15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="22">
+        <f>AVERAGE(C14,D14,E14)</f>
+        <v>6.0187316366529181E-3</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11"/>
+      <c r="B16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="14">
+        <f>STDEV(C14,D14,E14)</f>
+        <v>1.5507305359601336E-5</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11"/>
+      <c r="B17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="22">
+        <v>2.5888999999999999E-3</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mid-sems updates Commit by @arfazhxss on Thu 20 Jun 2024
</commit_message>
<xml_diff>
--- a/1 Summer 2024/1 CHEM 101 A01 B01/0 Labs/0 Past Submissions/Lab4/Book1.xlsx
+++ b/1 Summer 2024/1 CHEM 101 A01 B01/0 Labs/0 Past Submissions/Lab4/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arfaz/Desktop/ThirdYearEngineering/1 Summer 2024/1 CHEM 101 A01 B01/0 Labs/0 Past Submissions/Lab4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B75EAF-0E5D-1F48-A6DC-053FC8F98D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82610315-0EBD-EA42-BFF4-B2FA933CE698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{EB1F210C-BB4B-8141-9EF5-4BD3C8FB5D43}"/>
+    <workbookView minimized="1" xWindow="1000" yWindow="500" windowWidth="24600" windowHeight="15500" activeTab="2" xr2:uid="{EB1F210C-BB4B-8141-9EF5-4BD3C8FB5D43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Concentration (mmole/L)</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>Volume of acne cleanser used in the analysis (mL)</t>
-  </si>
-  <si>
-    <t>0.3mL</t>
   </si>
   <si>
     <t>Density of the acne cleanser used in the analysis (g/cm3)</t>
@@ -114,11 +111,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="168" formatCode="0.000000E+00"/>
-    <numFmt numFmtId="171" formatCode="0.000000000E+00"/>
-    <numFmt numFmtId="193" formatCode="0.0000000000"/>
-    <numFmt numFmtId="201" formatCode="0.00000000%"/>
-    <numFmt numFmtId="202" formatCode="0.000000000%"/>
+    <numFmt numFmtId="164" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.000000000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000%"/>
+    <numFmt numFmtId="168" formatCode="0.000000000%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -233,78 +230,72 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="202" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="193" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="193" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="193" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="193" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="201" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="201" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="201" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5114,8 +5105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17235206-13E0-F444-8427-08B45CA9E427}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="114" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5128,31 +5119,31 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <f>B3*1000</f>
+        <f t="shared" ref="B1:H1" si="0">B3*1000</f>
         <v>0.1142</v>
       </c>
       <c r="C1">
-        <f>C3*1000</f>
+        <f t="shared" si="0"/>
         <v>0.1142</v>
       </c>
       <c r="D1">
-        <f>D3*1000</f>
+        <f t="shared" si="0"/>
         <v>0.1142</v>
       </c>
       <c r="E1">
-        <f>E3*1000</f>
+        <f t="shared" si="0"/>
         <v>0.57099999999999995</v>
       </c>
       <c r="F1">
-        <f>F3*1000</f>
+        <f t="shared" si="0"/>
         <v>0.57099999999999995</v>
       </c>
       <c r="G1">
-        <f>G3*1000</f>
+        <f t="shared" si="0"/>
         <v>1.1419999999999999</v>
       </c>
       <c r="H1">
-        <f>H3*1000</f>
+        <f t="shared" si="0"/>
         <v>1.1419999999999999</v>
       </c>
     </row>
@@ -5184,7 +5175,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>1.142E-4</v>
@@ -5251,11 +5242,11 @@
         <v>5.0364468553992195E-4</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:D13" si="0">(C12-0.0298)/1179.8</f>
+        <f t="shared" ref="C13:D13" si="1">(C12-0.0298)/1179.8</f>
         <v>5.0110188167486007E-4</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.0279708425156799E-4</v>
       </c>
     </row>
@@ -5336,82 +5327,68 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C8A8A2-45DA-314B-8906-9F00CCC87B7A}">
-  <dimension ref="A2:F21"/>
+  <dimension ref="B3:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:E18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="12"/>
-    <col min="2" max="2" width="29" style="12" customWidth="1"/>
-    <col min="3" max="5" width="13.5" style="12" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="12"/>
+    <col min="1" max="1" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="29" style="6" customWidth="1"/>
+    <col min="3" max="5" width="13.5" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+    <row r="3" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E3" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="3" t="s">
+    <row r="4" spans="2:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="3">
         <v>0.96099999999999997</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="11"/>
+      <c r="E4" s="3">
+        <f>D4*D3</f>
+        <v>0.2883</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="7"/>
+    <row r="5" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="21"/>
       <c r="D5" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
+    <row r="6" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
       <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2" t="s">
+    </row>
+    <row r="7" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="C7" s="3">
         <v>0.624</v>
@@ -5422,212 +5399,168 @@
       <c r="E7" s="3">
         <v>0.623</v>
       </c>
-      <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
+    <row r="8" spans="2:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="19">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10">
         <f>(C7-0.0298)/1179.8</f>
         <v>5.0364468553992195E-4</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="10">
         <f t="shared" ref="D8:E8" si="0">(D7-0.0298)/1179.8</f>
         <v>5.0110188167486007E-4</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="10">
         <f t="shared" si="0"/>
         <v>5.0279708425156799E-4</v>
       </c>
-      <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
+    <row r="9" spans="2:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="18">
+        <v>11</v>
+      </c>
+      <c r="C9" s="9">
         <f>C8*(25/1000)</f>
         <v>1.2591117138498049E-5</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="9">
         <f>D8*(25/1000)</f>
         <v>1.2527547041871502E-5</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="9">
         <f>E8*(25/1000)</f>
         <v>1.2569927106289201E-5</v>
       </c>
-      <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
+    <row r="10" spans="2:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="18">
+        <v>12</v>
+      </c>
+      <c r="C10" s="9">
         <f>C9*138.1214</f>
         <v>1.7391027267333445E-3</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="9">
         <f t="shared" ref="D10:E10" si="1">D9*138.1214</f>
         <v>1.7303223359891504E-3</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="9">
         <f t="shared" si="1"/>
         <v>1.7361759298186131E-3</v>
       </c>
-      <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
+    <row r="11" spans="2:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="21">
+        <v>13</v>
+      </c>
+      <c r="C11" s="11">
         <f>C9/(0.3/1000)</f>
         <v>4.1970390461660165E-2</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="11">
         <f t="shared" ref="D11:E11" si="2">D9/(0.3/1000)</f>
         <v>4.1758490139571676E-2</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="11">
         <f t="shared" si="2"/>
         <v>4.1899757020964011E-2</v>
       </c>
-      <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
+    <row r="12" spans="2:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="13">
+        <v>14</v>
+      </c>
+      <c r="C12" s="7">
         <f>C11*(1/1000)</f>
         <v>4.1970390461660163E-5</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="7">
         <f t="shared" ref="D12:E12" si="3">D11*(1/1000)</f>
         <v>4.1758490139571679E-5</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="7">
         <f t="shared" si="3"/>
         <v>4.1899757020964015E-5</v>
       </c>
-      <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
+    <row r="13" spans="2:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="18">
+        <v>15</v>
+      </c>
+      <c r="C13" s="9">
         <f>C12*138.1214</f>
         <v>5.7970090891111478E-3</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="9">
         <f t="shared" ref="D13:E13" si="4">D12*138.1214</f>
         <v>5.7677411199638356E-3</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="9">
         <f t="shared" si="4"/>
         <v>5.7872530993953791E-3</v>
       </c>
-      <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
+    <row r="14" spans="2:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="17">
+        <v>16</v>
+      </c>
+      <c r="C14" s="8">
         <f>C13/$D4</f>
         <v>6.0322675224881873E-3</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="8">
         <f t="shared" ref="D14:E14" si="5">D13/$D4</f>
         <v>6.0018117793588302E-3</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="8">
         <f t="shared" si="5"/>
         <v>6.0221156081117369E-3</v>
       </c>
-      <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
+    <row r="15" spans="2:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="22">
+        <v>17</v>
+      </c>
+      <c r="C15" s="12">
         <f>AVERAGE(C14,D14,E14)</f>
         <v>6.0187316366529181E-3</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="11"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
+    <row r="16" spans="2:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="14">
+        <v>18</v>
+      </c>
+      <c r="C16" s="15">
         <f>STDEV(C14,D14,E14)</f>
         <v>1.5507305359601336E-5</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="11"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
     </row>
-    <row r="17" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
+    <row r="17" spans="2:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="12">
+        <v>2.5888999999999999E-3</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="2:5" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="22">
-        <v>2.5888999999999999E-3</v>
-      </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="C18" s="22">
+        <f>C15-D5</f>
+        <v>1.018731636652918E-3</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>